<commit_message>
added all main components etc.
</commit_message>
<xml_diff>
--- a/Current_BOM.xlsx
+++ b/Current_BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\ESE516-IOTEDGE\Shipwars_proj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\ESE516-IOTEDGE\Shipwars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C287B4C-7F26-49D2-A3C6-DD817B46EDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D77CA5E-A2CD-4A7C-81FE-675C8DCA6A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="315" windowWidth="18165" windowHeight="12390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="2" r:id="rId1"/>
@@ -44,32 +44,35 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Assume brightness of only 1 channel Led : neglect all other compnent power usage
 ======</t>
         </r>
       </text>
     </comment>
-    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="N10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>thumbstick not included
 ======</t>
         </r>
       </text>
     </comment>
-    <comment ref="G18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="G34" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>for 1 device
 ======</t>
@@ -81,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="123">
   <si>
     <t>Group Name</t>
   </si>
@@ -186,12 +189,6 @@
     <t>3.6V</t>
   </si>
   <si>
-    <t>Mini 2-Axis Analog Thumbstick</t>
-  </si>
-  <si>
-    <t>https://www.adafruit.com/product/3246</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -230,9 +227,6 @@
   </si>
   <si>
     <t>5V</t>
-  </si>
-  <si>
-    <t>2x ADC</t>
   </si>
   <si>
     <t>Power</t>
@@ -331,14 +325,150 @@
     <t>Y</t>
   </si>
   <si>
-    <t>N/A (will be provided)</t>
+    <t>Provided</t>
+  </si>
+  <si>
+    <t>External</t>
+  </si>
+  <si>
+    <t>COM-09032</t>
+  </si>
+  <si>
+    <t>Joystick, 2 - Axis Analog (Resistive) Output</t>
+  </si>
+  <si>
+    <t>Sparkfun</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/9110</t>
+  </si>
+  <si>
+    <t>2x ADC, 1XGPIO</t>
+  </si>
+  <si>
+    <t>N - import from SnapEDA to Schematics.SchLib</t>
+  </si>
+  <si>
+    <t>C1608X5R1A156M080AC</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>445-9117-2-ND</t>
+  </si>
+  <si>
+    <t>N - import from SnapEDA to CommonComponents.SchLib</t>
+  </si>
+  <si>
+    <t>6TPB470M</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>P16619CT-ND</t>
+  </si>
+  <si>
+    <t>GRM155R71A104KA01D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	
+490-6321-2-ND</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>Kemet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	C0603C105K8PACTU
+C0603C105K8PACTU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	
+399-C0603C105K8PAC7867TR-ND</t>
+  </si>
+  <si>
+    <t>DR127-2R2-R</t>
+  </si>
+  <si>
+    <t>513-1220-1-ND</t>
+  </si>
+  <si>
+    <t>Eaton</t>
+  </si>
+  <si>
+    <t>RC0603FR-07390KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	
+311-390KHRTR-ND</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>CRCW04022M15FKED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Vishay-Dale</t>
+  </si>
+  <si>
+    <t>541-2.15MLCT-ND</t>
+  </si>
+  <si>
+    <t>GRJ155R60J106ME11D</t>
+  </si>
+  <si>
+    <t>490-13211-1-ND</t>
+  </si>
+  <si>
+    <t>GRM188R60J226MEA0D</t>
+  </si>
+  <si>
+    <t>490-7611-2-ND</t>
+  </si>
+  <si>
+    <t>Wurth Elektronik</t>
+  </si>
+  <si>
+    <t>732-4177-1-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-07178KL</t>
+  </si>
+  <si>
+    <t>311-178KHRCT-ND</t>
+  </si>
+  <si>
+    <t>GRM155R71C104KA88D</t>
+  </si>
+  <si>
+    <t>any Generic Capacitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490-3261-2-ND </t>
+  </si>
+  <si>
+    <t>2SC1815</t>
+  </si>
+  <si>
+    <t>Central Semiconductor Corp</t>
+  </si>
+  <si>
+    <t>1514-2SC1815PBFREE-ND</t>
+  </si>
+  <si>
+    <t>any 2SC1815 equivalent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,8 +529,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -419,6 +556,12 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -429,10 +572,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -482,8 +626,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -697,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1008"/>
+  <dimension ref="A1:Z1024"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="P39" sqref="P39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -747,7 +899,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -804,10 +956,10 @@
         <v>9</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>10</v>
@@ -831,10 +983,10 @@
         <v>16</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="20.25" customHeight="1">
       <c r="A5" s="8" t="s">
         <v>17</v>
       </c>
@@ -842,7 +994,7 @@
         <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>19</v>
@@ -878,13 +1030,13 @@
         <v>41.04</v>
       </c>
       <c r="O5" s="2"/>
-      <c r="P5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="58.5" customHeight="1">
+      <c r="P5" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="70.5" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" s="3">
         <v>3954</v>
@@ -896,10 +1048,10 @@
         <v>25</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G6" s="2">
         <f>20*16</f>
@@ -927,10 +1079,10 @@
         <v>12.5</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="P6" t="s">
-        <v>22</v>
+        <v>42</v>
+      </c>
+      <c r="P6" s="19" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -938,7 +1090,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>30</v>
@@ -971,196 +1123,150 @@
         <v>22</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N7" s="3">
         <v>11.95</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="3"/>
+      <c r="B8" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="1:26" ht="57" customHeight="1">
+      <c r="A10" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="6">
-        <v>2765</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="C10" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J8" s="3">
-        <v>2</v>
-      </c>
-      <c r="K8" s="11">
-        <v>2.5</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="N8" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="O8" s="2"/>
-      <c r="P8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="17"/>
-      <c r="U9" s="17"/>
-      <c r="V9" s="17"/>
-      <c r="W9" s="17"/>
-      <c r="X9" s="17"/>
-      <c r="Y9" s="17"/>
-      <c r="Z9" s="17"/>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="F10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="18" t="s">
+        <v>84</v>
+      </c>
       <c r="J10" s="3">
         <v>2</v>
       </c>
-      <c r="K10" s="3">
-        <v>2.5299999999999998</v>
-      </c>
-      <c r="L10" s="3">
-        <v>1.41</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>57</v>
+      <c r="K10" s="11">
+        <v>3.95</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="20" t="s">
+        <v>83</v>
       </c>
       <c r="N10" s="3">
-        <v>118.8</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="P10" t="s">
-        <v>80</v>
+        <v>1.95</v>
+      </c>
+      <c r="O10" s="2"/>
+      <c r="P10" s="19" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="3">
-        <v>2</v>
-      </c>
-      <c r="K11" s="3">
-        <v>3.13</v>
-      </c>
-      <c r="L11" s="3">
-        <v>1.95</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="N11" s="3">
-        <v>58.8</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="P11" t="s">
-        <v>80</v>
-      </c>
+      <c r="A11" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="17"/>
+      <c r="Y11" s="17"/>
+      <c r="Z11" s="17"/>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -1169,42 +1275,42 @@
         <v>2</v>
       </c>
       <c r="K12" s="3">
-        <v>1.73</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="L12" s="3">
-        <v>0.97</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>22</v>
+        <v>1.41</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="N12" s="3">
+        <v>118.8</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>80</v>
+        <v>47</v>
+      </c>
+      <c r="P12" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>68</v>
+        <v>55</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>56</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>70</v>
+        <v>50</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1213,414 +1319,598 @@
         <v>2</v>
       </c>
       <c r="K13" s="3">
-        <v>6.49</v>
+        <v>3.13</v>
       </c>
       <c r="L13" s="3">
-        <v>5.75</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
+        <v>1.95</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="N13" s="3">
+        <v>58.8</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="P13" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="17"/>
-      <c r="U14" s="17"/>
-      <c r="V14" s="17"/>
-      <c r="W14" s="17"/>
-      <c r="X14" s="17"/>
-      <c r="Y14" s="17"/>
-      <c r="Z14" s="17"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3">
+        <v>1</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="19" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
       <c r="J15" s="3">
         <v>1</v>
       </c>
-      <c r="K15" s="3">
-        <v>0.61</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M15" s="3"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" t="s">
-        <v>80</v>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="19" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="B16" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3">
+        <v>1</v>
+      </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-    </row>
-    <row r="17" spans="1:15" ht="14.25" customHeight="1">
+      <c r="M16" s="5"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="14.25" customHeight="1">
       <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="B17" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>92</v>
+      </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3">
+        <v>1</v>
+      </c>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-    </row>
-    <row r="18" spans="1:15" ht="14.25" customHeight="1">
-      <c r="E18" s="2"/>
-      <c r="F18" s="2" t="s">
+      <c r="M17" s="5"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A18" s="3"/>
+      <c r="B18" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3">
+        <v>1</v>
+      </c>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A19" s="3"/>
+      <c r="B19" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3">
+        <v>1</v>
+      </c>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A20" s="3"/>
+      <c r="B20" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3">
+        <v>2</v>
+      </c>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="G18" s="2">
-        <f>G5+G6*2+G7</f>
-        <v>870.55</v>
-      </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2">
-        <f>K5*J5+K6*J6+K7*J7+K8*J8+J10*K10+J11*K11+J12*K12+J13*K13</f>
-        <v>117.78</v>
-      </c>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-    </row>
-    <row r="19" spans="1:15" ht="14.25" customHeight="1">
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-    </row>
-    <row r="20" spans="1:15" ht="14.25" customHeight="1">
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-    </row>
-    <row r="21" spans="1:15" ht="14.25" customHeight="1">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-    </row>
-    <row r="22" spans="1:15" ht="14.25" customHeight="1">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-    </row>
-    <row r="23" spans="1:15" ht="14.25" customHeight="1">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+    </row>
+    <row r="21" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A21" s="3"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="19"/>
+    </row>
+    <row r="22" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A22" s="3"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+    </row>
+    <row r="23" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A23" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-    </row>
-    <row r="24" spans="1:15" ht="14.25" customHeight="1">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-    </row>
-    <row r="25" spans="1:15" ht="14.25" customHeight="1">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-    </row>
-    <row r="26" spans="1:15" ht="14.25" customHeight="1">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-    </row>
-    <row r="27" spans="1:15" ht="14.25" customHeight="1">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-    </row>
-    <row r="28" spans="1:15" ht="14.25" customHeight="1">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
-    </row>
-    <row r="29" spans="1:15" ht="14.25" customHeight="1">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="J23" s="3">
+        <v>2</v>
+      </c>
+      <c r="K23" s="3">
+        <v>1.73</v>
+      </c>
+      <c r="L23" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A24" s="3"/>
+      <c r="B24" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A25" s="3"/>
+      <c r="B25" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A26" s="3"/>
+      <c r="B26" s="18">
+        <v>744311100</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A27" s="3"/>
+      <c r="B27" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+    </row>
+    <row r="29" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A29" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
+      <c r="J29" s="3">
+        <v>2</v>
+      </c>
+      <c r="K29" s="3">
+        <v>6.49</v>
+      </c>
+      <c r="L29" s="3">
+        <v>5.75</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
-    </row>
-    <row r="30" spans="1:15" ht="14.25" customHeight="1">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-    </row>
-    <row r="31" spans="1:15" ht="14.25" customHeight="1">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
+      <c r="P29" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A30" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="17"/>
+      <c r="Q30" s="17"/>
+      <c r="R30" s="17"/>
+      <c r="S30" s="17"/>
+      <c r="T30" s="17"/>
+      <c r="U30" s="17"/>
+      <c r="V30" s="17"/>
+      <c r="W30" s="17"/>
+      <c r="X30" s="17"/>
+      <c r="Y30" s="17"/>
+      <c r="Z30" s="17"/>
+    </row>
+    <row r="31" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A31" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
+      <c r="J31" s="3">
+        <v>1</v>
+      </c>
+      <c r="K31" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M31" s="3"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
-    </row>
-    <row r="32" spans="1:15" ht="14.25" customHeight="1">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
+      <c r="P31" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A32" s="3"/>
+      <c r="B32" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
       <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
+      <c r="O32" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="P32" s="19" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="33" spans="1:15" ht="14.25" customHeight="1">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
     </row>
     <row r="34" spans="1:15" ht="14.25" customHeight="1">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
       <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
+      <c r="F34" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G34" s="2">
+        <f>G5+G6*2+G7</f>
+        <v>870.55</v>
+      </c>
       <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
+      <c r="I34" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
+      <c r="K34" s="2">
+        <f>K5*J5+K6*J6+K7*J7+K10*J10+J12*K12+J13*K13+J23*K23+J29*K29</f>
+        <v>120.68</v>
+      </c>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
     </row>
     <row r="35" spans="1:15" ht="14.25" customHeight="1">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -1634,10 +1924,6 @@
       <c r="O35" s="2"/>
     </row>
     <row r="36" spans="1:15" ht="14.25" customHeight="1">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -18174,14 +18460,286 @@
       <c r="N1008" s="2"/>
       <c r="O1008" s="2"/>
     </row>
+    <row r="1009" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A1009" s="2"/>
+      <c r="B1009" s="2"/>
+      <c r="C1009" s="2"/>
+      <c r="D1009" s="2"/>
+      <c r="E1009" s="2"/>
+      <c r="F1009" s="2"/>
+      <c r="G1009" s="2"/>
+      <c r="H1009" s="2"/>
+      <c r="I1009" s="2"/>
+      <c r="J1009" s="2"/>
+      <c r="K1009" s="2"/>
+      <c r="L1009" s="2"/>
+      <c r="M1009" s="2"/>
+      <c r="N1009" s="2"/>
+      <c r="O1009" s="2"/>
+    </row>
+    <row r="1010" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A1010" s="2"/>
+      <c r="B1010" s="2"/>
+      <c r="C1010" s="2"/>
+      <c r="D1010" s="2"/>
+      <c r="E1010" s="2"/>
+      <c r="F1010" s="2"/>
+      <c r="G1010" s="2"/>
+      <c r="H1010" s="2"/>
+      <c r="I1010" s="2"/>
+      <c r="J1010" s="2"/>
+      <c r="K1010" s="2"/>
+      <c r="L1010" s="2"/>
+      <c r="M1010" s="2"/>
+      <c r="N1010" s="2"/>
+      <c r="O1010" s="2"/>
+    </row>
+    <row r="1011" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A1011" s="2"/>
+      <c r="B1011" s="2"/>
+      <c r="C1011" s="2"/>
+      <c r="D1011" s="2"/>
+      <c r="E1011" s="2"/>
+      <c r="F1011" s="2"/>
+      <c r="G1011" s="2"/>
+      <c r="H1011" s="2"/>
+      <c r="I1011" s="2"/>
+      <c r="J1011" s="2"/>
+      <c r="K1011" s="2"/>
+      <c r="L1011" s="2"/>
+      <c r="M1011" s="2"/>
+      <c r="N1011" s="2"/>
+      <c r="O1011" s="2"/>
+    </row>
+    <row r="1012" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A1012" s="2"/>
+      <c r="B1012" s="2"/>
+      <c r="C1012" s="2"/>
+      <c r="D1012" s="2"/>
+      <c r="E1012" s="2"/>
+      <c r="F1012" s="2"/>
+      <c r="G1012" s="2"/>
+      <c r="H1012" s="2"/>
+      <c r="I1012" s="2"/>
+      <c r="J1012" s="2"/>
+      <c r="K1012" s="2"/>
+      <c r="L1012" s="2"/>
+      <c r="M1012" s="2"/>
+      <c r="N1012" s="2"/>
+      <c r="O1012" s="2"/>
+    </row>
+    <row r="1013" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A1013" s="2"/>
+      <c r="B1013" s="2"/>
+      <c r="C1013" s="2"/>
+      <c r="D1013" s="2"/>
+      <c r="E1013" s="2"/>
+      <c r="F1013" s="2"/>
+      <c r="G1013" s="2"/>
+      <c r="H1013" s="2"/>
+      <c r="I1013" s="2"/>
+      <c r="J1013" s="2"/>
+      <c r="K1013" s="2"/>
+      <c r="L1013" s="2"/>
+      <c r="M1013" s="2"/>
+      <c r="N1013" s="2"/>
+      <c r="O1013" s="2"/>
+    </row>
+    <row r="1014" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A1014" s="2"/>
+      <c r="B1014" s="2"/>
+      <c r="C1014" s="2"/>
+      <c r="D1014" s="2"/>
+      <c r="E1014" s="2"/>
+      <c r="F1014" s="2"/>
+      <c r="G1014" s="2"/>
+      <c r="H1014" s="2"/>
+      <c r="I1014" s="2"/>
+      <c r="J1014" s="2"/>
+      <c r="K1014" s="2"/>
+      <c r="L1014" s="2"/>
+      <c r="M1014" s="2"/>
+      <c r="N1014" s="2"/>
+      <c r="O1014" s="2"/>
+    </row>
+    <row r="1015" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A1015" s="2"/>
+      <c r="B1015" s="2"/>
+      <c r="C1015" s="2"/>
+      <c r="D1015" s="2"/>
+      <c r="E1015" s="2"/>
+      <c r="F1015" s="2"/>
+      <c r="G1015" s="2"/>
+      <c r="H1015" s="2"/>
+      <c r="I1015" s="2"/>
+      <c r="J1015" s="2"/>
+      <c r="K1015" s="2"/>
+      <c r="L1015" s="2"/>
+      <c r="M1015" s="2"/>
+      <c r="N1015" s="2"/>
+      <c r="O1015" s="2"/>
+    </row>
+    <row r="1016" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A1016" s="2"/>
+      <c r="B1016" s="2"/>
+      <c r="C1016" s="2"/>
+      <c r="D1016" s="2"/>
+      <c r="E1016" s="2"/>
+      <c r="F1016" s="2"/>
+      <c r="G1016" s="2"/>
+      <c r="H1016" s="2"/>
+      <c r="I1016" s="2"/>
+      <c r="J1016" s="2"/>
+      <c r="K1016" s="2"/>
+      <c r="L1016" s="2"/>
+      <c r="M1016" s="2"/>
+      <c r="N1016" s="2"/>
+      <c r="O1016" s="2"/>
+    </row>
+    <row r="1017" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A1017" s="2"/>
+      <c r="B1017" s="2"/>
+      <c r="C1017" s="2"/>
+      <c r="D1017" s="2"/>
+      <c r="E1017" s="2"/>
+      <c r="F1017" s="2"/>
+      <c r="G1017" s="2"/>
+      <c r="H1017" s="2"/>
+      <c r="I1017" s="2"/>
+      <c r="J1017" s="2"/>
+      <c r="K1017" s="2"/>
+      <c r="L1017" s="2"/>
+      <c r="M1017" s="2"/>
+      <c r="N1017" s="2"/>
+      <c r="O1017" s="2"/>
+    </row>
+    <row r="1018" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A1018" s="2"/>
+      <c r="B1018" s="2"/>
+      <c r="C1018" s="2"/>
+      <c r="D1018" s="2"/>
+      <c r="E1018" s="2"/>
+      <c r="F1018" s="2"/>
+      <c r="G1018" s="2"/>
+      <c r="H1018" s="2"/>
+      <c r="I1018" s="2"/>
+      <c r="J1018" s="2"/>
+      <c r="K1018" s="2"/>
+      <c r="L1018" s="2"/>
+      <c r="M1018" s="2"/>
+      <c r="N1018" s="2"/>
+      <c r="O1018" s="2"/>
+    </row>
+    <row r="1019" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A1019" s="2"/>
+      <c r="B1019" s="2"/>
+      <c r="C1019" s="2"/>
+      <c r="D1019" s="2"/>
+      <c r="E1019" s="2"/>
+      <c r="F1019" s="2"/>
+      <c r="G1019" s="2"/>
+      <c r="H1019" s="2"/>
+      <c r="I1019" s="2"/>
+      <c r="J1019" s="2"/>
+      <c r="K1019" s="2"/>
+      <c r="L1019" s="2"/>
+      <c r="M1019" s="2"/>
+      <c r="N1019" s="2"/>
+      <c r="O1019" s="2"/>
+    </row>
+    <row r="1020" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A1020" s="2"/>
+      <c r="B1020" s="2"/>
+      <c r="C1020" s="2"/>
+      <c r="D1020" s="2"/>
+      <c r="E1020" s="2"/>
+      <c r="F1020" s="2"/>
+      <c r="G1020" s="2"/>
+      <c r="H1020" s="2"/>
+      <c r="I1020" s="2"/>
+      <c r="J1020" s="2"/>
+      <c r="K1020" s="2"/>
+      <c r="L1020" s="2"/>
+      <c r="M1020" s="2"/>
+      <c r="N1020" s="2"/>
+      <c r="O1020" s="2"/>
+    </row>
+    <row r="1021" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A1021" s="2"/>
+      <c r="B1021" s="2"/>
+      <c r="C1021" s="2"/>
+      <c r="D1021" s="2"/>
+      <c r="E1021" s="2"/>
+      <c r="F1021" s="2"/>
+      <c r="G1021" s="2"/>
+      <c r="H1021" s="2"/>
+      <c r="I1021" s="2"/>
+      <c r="J1021" s="2"/>
+      <c r="K1021" s="2"/>
+      <c r="L1021" s="2"/>
+      <c r="M1021" s="2"/>
+      <c r="N1021" s="2"/>
+      <c r="O1021" s="2"/>
+    </row>
+    <row r="1022" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A1022" s="2"/>
+      <c r="B1022" s="2"/>
+      <c r="C1022" s="2"/>
+      <c r="D1022" s="2"/>
+      <c r="E1022" s="2"/>
+      <c r="F1022" s="2"/>
+      <c r="G1022" s="2"/>
+      <c r="H1022" s="2"/>
+      <c r="I1022" s="2"/>
+      <c r="J1022" s="2"/>
+      <c r="K1022" s="2"/>
+      <c r="L1022" s="2"/>
+      <c r="M1022" s="2"/>
+      <c r="N1022" s="2"/>
+      <c r="O1022" s="2"/>
+    </row>
+    <row r="1023" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A1023" s="2"/>
+      <c r="B1023" s="2"/>
+      <c r="C1023" s="2"/>
+      <c r="D1023" s="2"/>
+      <c r="E1023" s="2"/>
+      <c r="F1023" s="2"/>
+      <c r="G1023" s="2"/>
+      <c r="H1023" s="2"/>
+      <c r="I1023" s="2"/>
+      <c r="J1023" s="2"/>
+      <c r="K1023" s="2"/>
+      <c r="L1023" s="2"/>
+      <c r="M1023" s="2"/>
+      <c r="N1023" s="2"/>
+      <c r="O1023" s="2"/>
+    </row>
+    <row r="1024" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A1024" s="2"/>
+      <c r="B1024" s="2"/>
+      <c r="C1024" s="2"/>
+      <c r="D1024" s="2"/>
+      <c r="E1024" s="2"/>
+      <c r="F1024" s="2"/>
+      <c r="G1024" s="2"/>
+      <c r="H1024" s="2"/>
+      <c r="I1024" s="2"/>
+      <c r="J1024" s="2"/>
+      <c r="K1024" s="2"/>
+      <c r="L1024" s="2"/>
+      <c r="M1024" s="2"/>
+      <c r="N1024" s="2"/>
+      <c r="O1024" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M5" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="M6" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
     <hyperlink ref="M7" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="M8" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="M10" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="M11" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="M10" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="M12" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="M13" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>